<commit_message>
Update files of automation
</commit_message>
<xml_diff>
--- a/First Sprint/Admin Registration story_2024_09_21_Execution.xlsx
+++ b/First Sprint/Admin Registration story_2024_09_21_Execution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\my cv files\First Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="149">
   <si>
     <t>Project Name</t>
   </si>
@@ -128,219 +128,20 @@
     <t>Admin-reg_SID_01_TC_01</t>
   </si>
   <si>
-    <t>Check response for entering First name</t>
-  </si>
-  <si>
-    <t>1. Open Site with it's url</t>
-  </si>
-  <si>
     <t>User should be able to see the page</t>
-  </si>
-  <si>
-    <t>2. Registration form must shown</t>
-  </si>
-  <si>
-    <t>Registration form should be displayed</t>
-  </si>
-  <si>
-    <t>3. First name field must be there 
-to input value</t>
-  </si>
-  <si>
-    <t>User should be able to see the first name field</t>
-  </si>
-  <si>
-    <t>4. Enter data in first name field</t>
-  </si>
-  <si>
-    <t>Admin1</t>
-  </si>
-  <si>
-    <t>User should be able to enter value</t>
-  </si>
-  <si>
-    <t>5. Save button must be there and
- clickable</t>
-  </si>
-  <si>
-    <t>User should be able to see the save button
- and click</t>
-  </si>
-  <si>
-    <t>6. Click on save button</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_02</t>
-  </si>
-  <si>
-    <t>Check response for making empty in First name field</t>
-  </si>
-  <si>
-    <t>1.  open site with it's url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. First name field must be there 
-to input value </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. click in that field and make that
- field empty </t>
-  </si>
-  <si>
-    <t>User should be able to leave first name field
- empty with error message</t>
-  </si>
-  <si>
-    <t>User should be able to see the save button 
-and click</t>
-  </si>
-  <si>
-    <t>6. Click on Save button</t>
   </si>
   <si>
     <t>User data should not be stored in database and
  user should be able to see error message</t>
   </si>
   <si>
-    <t>Admin-reg_SID_01_TC_03</t>
-  </si>
-  <si>
-    <t>Check response for entering last name</t>
-  </si>
-  <si>
-    <t>3. Last name field must be there 
-to input value</t>
-  </si>
-  <si>
-    <t>User should be able to see the last name field</t>
-  </si>
-  <si>
-    <t>4. Enter data in last name field</t>
-  </si>
-  <si>
-    <t>Neupane</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_04</t>
-  </si>
-  <si>
-    <t>Check response for making empty in last name field</t>
-  </si>
-  <si>
-    <t>1. open site with it's url</t>
-  </si>
-  <si>
-    <t>User should be able to leave last name field
- empty with error message</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_05</t>
-  </si>
-  <si>
-    <t>Check response for entering email</t>
-  </si>
-  <si>
-    <t>3. Email field must be there 
-to input value</t>
-  </si>
-  <si>
-    <t>User should be able to see the email field</t>
-  </si>
-  <si>
-    <t>4. Enter data in email field</t>
-  </si>
-  <si>
-    <t>nothing.nothing@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_06</t>
-  </si>
-  <si>
-    <t>Check response for making email field empty</t>
-  </si>
-  <si>
-    <t>User should be able to leave email field
- empty with error message</t>
-  </si>
-  <si>
-    <t>5. save button must be there and 
-clickable</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_07</t>
-  </si>
-  <si>
-    <t>Check response for making password field empty</t>
-  </si>
-  <si>
-    <t>3. Password field must be there 
-to input value</t>
-  </si>
-  <si>
-    <t>User should be able to see the password field</t>
-  </si>
-  <si>
-    <t>User should be able to leave password field
- empty with error message</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_08</t>
-  </si>
-  <si>
-    <t>Check response for entering password</t>
-  </si>
-  <si>
-    <t>4. Enter data in password field</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_09</t>
-  </si>
-  <si>
-    <t>Check response for entering phone number</t>
-  </si>
-  <si>
-    <t>3. Phone number field must be there to input value</t>
-  </si>
-  <si>
-    <t>User should be able to see the phone number field</t>
-  </si>
-  <si>
-    <t>4. Enter data in phone number field</t>
-  </si>
-  <si>
-    <t>Admin-reg_SID_01_TC_10</t>
-  </si>
-  <si>
-    <t>Check response for making phone number field empty</t>
-  </si>
-  <si>
-    <t>User should be able to leave phone number field empty with error message</t>
-  </si>
-  <si>
-    <t>5. save button must be there and
- clickable</t>
-  </si>
-  <si>
     <t>Admin-reg_SID_02</t>
   </si>
   <si>
     <t>Verify Super admin role selection</t>
   </si>
   <si>
-    <t>Admin-reg_SID_02_TC_1</t>
-  </si>
-  <si>
     <t>Check response for selecting single role to new admin</t>
-  </si>
-  <si>
-    <t>3. Role assign field must be shown</t>
-  </si>
-  <si>
-    <t>User should be able to see the role assign field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Select single role for admin
-</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to select or assign 
@@ -353,31 +154,13 @@
     <t>Check response for selecting multiple role to new admin</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Select multiple roles for admin
-</t>
-  </si>
-  <si>
     <t>User should be able to select or assign 
 multiple roles</t>
   </si>
   <si>
-    <t>1.open site with it's url</t>
-  </si>
-  <si>
     <t>Check response for not selecting any role to new admin</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Don't Select any role for admin
-</t>
-  </si>
-  <si>
-    <t>User should be able to leave assign field and error should be shown</t>
-  </si>
-  <si>
-    <t>User should be able to see the button for 
-saving  and clickable</t>
-  </si>
-  <si>
     <t>Admin-reg_SID_03</t>
   </si>
   <si>
@@ -385,15 +168,6 @@
   </si>
   <si>
     <t>Check response for activation of admin user</t>
-  </si>
-  <si>
-    <t>3. Activation button must be there inside registration form</t>
-  </si>
-  <si>
-    <t>User should be able to see activate button</t>
-  </si>
-  <si>
-    <t>4. Click on activate button</t>
   </si>
   <si>
     <t>User should be able to click on activate
@@ -403,23 +177,10 @@
     <t>Check response for deactivation of admin user</t>
   </si>
   <si>
-    <t>3. De-activation button must be there</t>
-  </si>
-  <si>
-    <t>User should be able to see de-activate button</t>
-  </si>
-  <si>
-    <t>4. Click on De-activate button</t>
-  </si>
-  <si>
     <t>User should be able to click on de-activate
  button</t>
   </si>
   <si>
-    <t>5. Button must be there for saving 
-data and clickable</t>
-  </si>
-  <si>
     <t>https://qaecoma.bishalkarki.xyz/admin123/index.php?
 controller=AdminEmployees&amp;addemployee&amp;token=fe94438651e856e9ec135c50401898c9</t>
   </si>
@@ -430,40 +191,13 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>User is able to leave empty
- field but without error message</t>
-  </si>
-  <si>
-    <t>Partially pass</t>
-  </si>
-  <si>
-    <t>Partially Pass</t>
-  </si>
-  <si>
-    <t>User is not able to see the
- phone number field</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Blocked</t>
-  </si>
-  <si>
-    <t>Dependency with above step</t>
-  </si>
-  <si>
     <t>User is not able to select or assign multiple roles</t>
   </si>
   <si>
-    <t>User is able to leave assign
- field but error message is not shown</t>
-  </si>
-  <si>
     <t>Not as expected</t>
-  </si>
-  <si>
-    <t>User is able to click it</t>
   </si>
   <si>
     <t>There is yes/no button for
@@ -482,42 +216,307 @@
     <t>Admin-reg_SID_03_TC_01</t>
   </si>
   <si>
-    <t>Check response for entering all data</t>
-  </si>
-  <si>
-    <t>3. Insert data in all field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Click on save button </t>
-  </si>
-  <si>
-    <t>4. There must be save button and must be clickable</t>
-  </si>
-  <si>
-    <t>Firstname:admin1
-Last name: Neupane
-Email: hello@gmail.com
-Phone number: 9876543219
-Password:hello@gmail.com</t>
-  </si>
-  <si>
-    <t>User should be able to insert all data</t>
-  </si>
-  <si>
-    <t>All data should be stored in database by being registration successful</t>
-  </si>
-  <si>
-    <t>User should be able to see the save button and click</t>
-  </si>
-  <si>
     <t>Executed by</t>
+  </si>
+  <si>
+    <t>1. Open admin registration page</t>
+  </si>
+  <si>
+    <t>User should be able to enter data in first name field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to leave first name field
+ empty </t>
+  </si>
+  <si>
+    <t>First Name: Admin11</t>
+  </si>
+  <si>
+    <t>First Name:</t>
+  </si>
+  <si>
+    <t>User should be able to enter data in last name field</t>
+  </si>
+  <si>
+    <t>User should be able to enter data in phone number field</t>
+  </si>
+  <si>
+    <t>User should be able to enter data in Email field</t>
+  </si>
+  <si>
+    <t>User should be able to enter data in password field</t>
+  </si>
+  <si>
+    <t>Phone number field is missing</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Phone number field is missing inside admin registration page so this test case is fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response for making empty in First name field </t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_02_TC_01</t>
+  </si>
+  <si>
+    <t>2. Locate first name field</t>
+  </si>
+  <si>
+    <t>3. Enter first name inside first name field</t>
+  </si>
+  <si>
+    <t>4. Locate last name field</t>
+  </si>
+  <si>
+    <t>The First Name field should be visible and ready for input</t>
+  </si>
+  <si>
+    <t>The Last Name field should be visible and ready for input</t>
+  </si>
+  <si>
+    <t>5. Enter last name inside last name field</t>
+  </si>
+  <si>
+    <t>6. Locate email field</t>
+  </si>
+  <si>
+    <t>Email field should be visible and ready for input</t>
+  </si>
+  <si>
+    <t>7. Enter Email inside email field</t>
+  </si>
+  <si>
+    <t>8. Locate password field</t>
+  </si>
+  <si>
+    <t>Password field should be visible and ready to input</t>
+  </si>
+  <si>
+    <t>9. Enter password inside password field</t>
+  </si>
+  <si>
+    <t>11. Enter phone number inside phone number field</t>
+  </si>
+  <si>
+    <t>10. Locate phone number field</t>
+  </si>
+  <si>
+    <t>Phone number field should be visible and ready to input</t>
+  </si>
+  <si>
+    <t>2. Locate role assign field</t>
+  </si>
+  <si>
+    <t>Role assign field should be visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Select single role for admin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Select multiple role for admin
+</t>
+  </si>
+  <si>
+    <t>2. Locate activation button</t>
+  </si>
+  <si>
+    <t>Activation button should be visible</t>
+  </si>
+  <si>
+    <t>3. Click on activate button</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_03_TC_02</t>
+  </si>
+  <si>
+    <t>2. Locate deactivation button</t>
+  </si>
+  <si>
+    <t>Deactivation button should be visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is yes/no button for
+ activation and deactivation, which means the same as expected </t>
+  </si>
+  <si>
+    <t>User is able to click into it</t>
+  </si>
+  <si>
+    <t>3. Click on De-activate button</t>
+  </si>
+  <si>
+    <t>Verify empty data in field</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Make first name field empty </t>
+  </si>
+  <si>
+    <t>3. Enter data in all other field</t>
+  </si>
+  <si>
+    <t>User should be able to insert data</t>
+  </si>
+  <si>
+    <t>Phone number field is missing so this step is in hold status</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
+    <t>Dependent with above step</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response for making empty in Last name field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Make Last name field empty </t>
+  </si>
+  <si>
+    <t>Last Name:</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response for making empty in Email field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Make email field empty </t>
+  </si>
+  <si>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>First Name: Admin100
+Last Name: Neupane
+Password:test123
+Phone Number:9834567890
+Assign role: "Salesman"
+Activation Mode: "Yes"</t>
+  </si>
+  <si>
+    <t>4. Click on Save button</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response for making empty in Password field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Make Password field empty </t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response for making empty in Phone number field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Make Phone number field empty </t>
+  </si>
+  <si>
+    <t>Phone number:</t>
+  </si>
+  <si>
+    <t>Not As expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to leave phone number field
+ empty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone number field is missing </t>
+  </si>
+  <si>
+    <t>Admin-reg_SID_04_TC_06</t>
+  </si>
+  <si>
+    <t>2. Leave the role unselected</t>
+  </si>
+  <si>
+    <t>Assign role:</t>
+  </si>
+  <si>
+    <t>User should be able to leave role field unselected</t>
+  </si>
+  <si>
+    <t>Last Name: Neupane</t>
+  </si>
+  <si>
+    <t>Email: test123@gmail.com</t>
+  </si>
+  <si>
+    <t>Password: test123</t>
+  </si>
+  <si>
+    <t>Phone Number: 9834567890</t>
+  </si>
+  <si>
+    <t>Check response for entering First name, last name, email, 
+password and phone number</t>
+  </si>
+  <si>
+    <t>Assign role: "Salesman"</t>
+  </si>
+  <si>
+    <t>Assign role 1: "Salesman"
+Assign role 2: "Logistician"</t>
+  </si>
+  <si>
+    <t>Last Name: Neupane
+Email: testing123@gmail.com
+Password:test123
+Phone Number:9834567890
+Assign role: "Salesman"</t>
+  </si>
+  <si>
+    <t>First Name: Admin100
+Email: testing123@gmail.com
+Password:test123
+Phone Number:9834567890
+Assign role: "Salesman"</t>
+  </si>
+  <si>
+    <t>First Name: Admin100
+Last Name: Neupane
+Email:test123@gmail.com
+Phone Number:9834567890
+Assign role: "Salesman"</t>
+  </si>
+  <si>
+    <t>First Name: Admin100
+Last Name: Neupane
+Email:test123@gmail.com
+Password:test123
+Assign role: "Salesman"</t>
+  </si>
+  <si>
+    <t>First Name: Admin100
+Last Name: Neupane
+Email:test123@gmail.com
+Password:test123
+Phone Number: 9834567890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,12 +533,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -582,19 +575,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,6 +583,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -647,9 +640,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -690,18 +683,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -709,21 +698,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:J1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -955,11 +966,11 @@
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.140625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="52.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
+    <col min="7" max="7" width="60.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
     <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -976,8 +987,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>123</v>
+      <c r="B2" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="J2" s="3"/>
     </row>
@@ -1071,7 +1082,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -1082,8 +1093,8 @@
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="33" t="s">
-        <v>130</v>
+      <c r="B14" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="J14" s="3"/>
     </row>
@@ -1129,7 +1140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
@@ -1139,1494 +1150,1234 @@
       <c r="C18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="20"/>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="29"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="29"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="29"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="29"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E25" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" s="29"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E26" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="29"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E27" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E28" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="29"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E32" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="29"/>
+      <c r="J32" s="20"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="20"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="20"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E36" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E39" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I39" s="34"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E40" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I40" s="34"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H41" s="20"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E43" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E44" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I44" s="29"/>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I45" s="28"/>
+      <c r="J45" s="20"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J46" s="20"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E47" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" t="s">
+        <v>51</v>
+      </c>
+      <c r="I47" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J47" s="20"/>
+    </row>
+    <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="E48" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="E49" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I49" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="12"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51" t="s">
+        <v>51</v>
+      </c>
+      <c r="I51" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" t="s">
+        <v>115</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" t="s">
+        <v>51</v>
+      </c>
+      <c r="I52" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I53" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I54" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H56" t="s">
+        <v>51</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F57" t="s">
+        <v>119</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" t="s">
+        <v>51</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I58" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="12"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H61" t="s">
+        <v>51</v>
+      </c>
+      <c r="I61" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="F62" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" t="s">
-        <v>124</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E20" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" t="s">
-        <v>124</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="11" t="s">
+      <c r="G62" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I63" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J63" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I64" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="12"/>
+      <c r="G65" s="11"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H66" t="s">
+        <v>51</v>
+      </c>
+      <c r="I66" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H67" t="s">
+        <v>130</v>
+      </c>
+      <c r="I67" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I68" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I69" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="11"/>
+      <c r="G70" s="14"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H21" t="s">
-        <v>124</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="11"/>
-      <c r="G23" s="14"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="C24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" t="s">
-        <v>124</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="12" t="s">
+      <c r="E71" t="s">
+        <v>62</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="I71" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" t="s">
-        <v>124</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" t="s">
-        <v>124</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H31" t="s">
-        <v>124</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E32" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H32" t="s">
-        <v>124</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" t="s">
-        <v>124</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="I34" s="24"/>
-    </row>
-    <row r="35" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="11"/>
-      <c r="G35" s="14"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" t="s">
-        <v>124</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E37" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" t="s">
-        <v>124</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="3:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E38" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="H38" t="s">
-        <v>124</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="3:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="12" t="s">
+    </row>
+    <row r="72" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F72" t="s">
+        <v>135</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H72" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I39" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="J39" s="13"/>
-    </row>
-    <row r="40" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E40" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I40" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H41" t="s">
-        <v>124</v>
-      </c>
-      <c r="I41" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H42" t="s">
-        <v>124</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H43" t="s">
-        <v>124</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="3:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E44" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H44" t="s">
-        <v>124</v>
-      </c>
-      <c r="I44" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H45" t="s">
-        <v>124</v>
-      </c>
-      <c r="I45" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E47" s="11"/>
-      <c r="G47" s="14"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="13"/>
-    </row>
-    <row r="48" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="11" t="s">
+      <c r="I72" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I73" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H48" t="s">
-        <v>124</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E49" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" t="s">
-        <v>124</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H50" t="s">
-        <v>124</v>
-      </c>
-      <c r="I50" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E51" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="H51" t="s">
-        <v>124</v>
-      </c>
-      <c r="I51" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J51" s="13"/>
-    </row>
-    <row r="52" spans="3:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E52" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" t="s">
-        <v>124</v>
-      </c>
-      <c r="I52" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E53" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H53" t="s">
-        <v>124</v>
-      </c>
-      <c r="I53" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H54" t="s">
-        <v>124</v>
-      </c>
-      <c r="I54" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E55" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H55" t="s">
-        <v>124</v>
-      </c>
-      <c r="I55" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E56" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="H56" t="s">
-        <v>124</v>
-      </c>
-      <c r="I56" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="3:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E57" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="J57" s="13"/>
-    </row>
-    <row r="58" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E58" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H58" t="s">
-        <v>124</v>
-      </c>
-      <c r="I58" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E59" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G59" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H59" t="s">
-        <v>124</v>
-      </c>
-      <c r="I59" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="3:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H60" t="s">
-        <v>124</v>
-      </c>
-      <c r="I60" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E61" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" t="s">
-        <v>124</v>
-      </c>
-      <c r="I61" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="3:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E62" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H62" t="s">
-        <v>124</v>
-      </c>
-      <c r="I62" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E63" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F63" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H63" t="s">
-        <v>124</v>
-      </c>
-      <c r="I63" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J63" s="3"/>
-    </row>
-    <row r="64" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="3"/>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E65" s="11"/>
-      <c r="G65" s="14"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="13"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H66" t="s">
-        <v>124</v>
-      </c>
-      <c r="I66" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J66" s="3"/>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E67" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H67" t="s">
-        <v>124</v>
-      </c>
-      <c r="I67" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J67" s="3"/>
-    </row>
-    <row r="68" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E68" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H68" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I68" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="J68" s="3"/>
-    </row>
-    <row r="69" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E69" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F69" s="11">
-        <v>9854367432</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I69" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J69" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E70" s="12"/>
-      <c r="G70" s="12"/>
-      <c r="J70" s="3"/>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E71" s="11"/>
-      <c r="G71" s="14"/>
-      <c r="J71" s="13"/>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H72" t="s">
-        <v>124</v>
-      </c>
-      <c r="I72" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J72" s="3"/>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E73" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G73" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H73" t="s">
-        <v>124</v>
-      </c>
-      <c r="I73" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J73" s="3"/>
-    </row>
-    <row r="74" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E74" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H74" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I74" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E75" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="H75" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I75" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J75" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E76" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H76" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I76" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J76" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E77" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H77" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I77" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J77" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H78" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I78" s="24" t="s">
-        <v>125</v>
-      </c>
+      <c r="J73" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G74" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I74" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="11"/>
+      <c r="G76" s="14"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="11"/>
+      <c r="G77" s="15"/>
+      <c r="I77" s="23"/>
+      <c r="J77" s="13"/>
+    </row>
+    <row r="78" spans="3:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="11"/>
+      <c r="G78" s="15"/>
+      <c r="I78" s="23"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E79" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H79" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I79" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="79" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="12"/>
+      <c r="G79" s="11"/>
+      <c r="I79" s="23"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E80" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H80" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I80" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E81" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="H81" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I81" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E82" s="15"/>
-      <c r="G82" s="15"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="24"/>
+    <row r="80" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="13"/>
+    </row>
+    <row r="81" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E81" s="14"/>
+      <c r="G81" s="15"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="13"/>
+    </row>
+    <row r="82" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="12"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="23"/>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="I83" s="24"/>
-      <c r="J83" s="13"/>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E84" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H84" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I84" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="83" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="11"/>
+      <c r="G84" s="14"/>
+      <c r="I84" s="23"/>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G85" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H85" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I85" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E86" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H86" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I86" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="85" spans="3:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="11"/>
+      <c r="G85" s="15"/>
+      <c r="I85" s="23"/>
+      <c r="J85" s="13"/>
+    </row>
+    <row r="86" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E86" s="11"/>
+      <c r="G86" s="15"/>
+      <c r="I86" s="23"/>
       <c r="J86" s="3"/>
     </row>
-    <row r="87" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E87" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G87" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H87" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="I87" s="30" t="s">
-        <v>130</v>
-      </c>
+    <row r="87" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E87" s="12"/>
+      <c r="G87" s="11"/>
+      <c r="I87" s="23"/>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E88" s="15"/>
-      <c r="G88" s="15"/>
-      <c r="J88" s="3"/>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="89" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E89" s="14"/>
       <c r="G89" s="14"/>
+      <c r="I89" s="23"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E90" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G90" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H90" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I90" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="90" spans="3:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="11"/>
+      <c r="I90" s="23"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E91" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G91" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H91" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I91" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="91" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="I91" s="23"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C92" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E92" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G92" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H92" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I92" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="92" spans="3:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E92" s="11"/>
+      <c r="G92" s="14"/>
+      <c r="I92" s="23"/>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E93" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H93" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="I93" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="J93" s="13"/>
-    </row>
-    <row r="94" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E94" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G94" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H94" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I94" s="31" t="s">
-        <v>125</v>
-      </c>
+    <row r="93" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="I93" s="23"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="3:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E94" s="12"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="23"/>
       <c r="J94" s="3"/>
     </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E95" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G95" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H95" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="I95" s="28" t="s">
-        <v>130</v>
-      </c>
+    <row r="95" spans="3:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="23"/>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C96" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G96" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H96" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I96" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="J96" s="3"/>
-    </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E97" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G97" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H97" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I97" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="J97" s="13"/>
-    </row>
-    <row r="98" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E98" s="14"/>
+    <row r="96" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E96" s="18"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="20"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="13"/>
+    </row>
+    <row r="97" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="27"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E99" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="G99" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="H99" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="I99" s="31" t="s">
-        <v>125</v>
-      </c>
+    <row r="99" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" s="11"/>
+      <c r="E99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="20"/>
+      <c r="I99" s="27"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E100" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G100" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H100" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="I100" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="J100" s="3"/>
-    </row>
-    <row r="101" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="20"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="13"/>
+    </row>
+    <row r="101" spans="3:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E101" s="15"/>
       <c r="G101" s="15"/>
+      <c r="H101" s="20"/>
       <c r="I101" s="27"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E102" s="14"/>
-      <c r="G102" s="14"/>
-      <c r="I102" s="32"/>
-      <c r="J102" s="13"/>
-    </row>
-    <row r="103" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E103" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G103" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H103" t="s">
-        <v>124</v>
-      </c>
-      <c r="I103" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E104" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G104" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H104" t="s">
-        <v>124</v>
-      </c>
-      <c r="I104" s="24" t="s">
-        <v>125</v>
-      </c>
+    <row r="102" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I102" s="23"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I103" s="23"/>
+      <c r="J103" s="13"/>
+    </row>
+    <row r="104" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I104" s="23"/>
       <c r="J104" s="13"/>
     </row>
-    <row r="105" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C105" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D105" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E105" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G105" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H105" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="I105" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J105" s="3"/>
-    </row>
-    <row r="106" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E106" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="G106" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H106" t="s">
-        <v>138</v>
-      </c>
-      <c r="I106" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="J106" s="3"/>
-    </row>
-    <row r="107" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E107" s="15"/>
-      <c r="G107" s="15"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="3"/>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B108" t="s">
-        <v>140</v>
-      </c>
-      <c r="C108" s="23" t="s">
+    <row r="105" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="23"/>
+    </row>
+    <row r="106" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="I106" s="23"/>
+    </row>
+    <row r="107" spans="3:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="I107" s="25"/>
+    </row>
+    <row r="108" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I108" s="23"/>
+    </row>
+    <row r="109" spans="3:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I109" s="23"/>
+      <c r="J109" s="3"/>
+    </row>
+    <row r="110" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I110" s="23"/>
+      <c r="J110" s="13"/>
+    </row>
+    <row r="111" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I111" s="23"/>
+      <c r="J111" s="3"/>
+    </row>
+    <row r="112" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E112" s="15"/>
+      <c r="G112" s="15"/>
+      <c r="I112" s="23"/>
+      <c r="J112" s="13"/>
+    </row>
+    <row r="113" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E113" s="12"/>
+      <c r="G113" s="11"/>
+      <c r="I113" s="23"/>
+      <c r="J113" s="3"/>
+    </row>
+    <row r="114" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="I114" s="23"/>
+      <c r="J114" s="3"/>
+    </row>
+    <row r="115" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F115" s="20"/>
+      <c r="G115" s="15"/>
+      <c r="I115" s="23"/>
+      <c r="J115" s="3"/>
+    </row>
+    <row r="116" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B116" t="s">
+        <v>59</v>
+      </c>
+      <c r="C116" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D108" t="s">
-        <v>142</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G108" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H108" t="s">
-        <v>124</v>
-      </c>
-      <c r="I108" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J108" s="13"/>
-    </row>
-    <row r="109" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E109" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G109" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H109" t="s">
-        <v>124</v>
-      </c>
-      <c r="I109" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J109" s="3"/>
-    </row>
-    <row r="110" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E110" t="s">
-        <v>143</v>
-      </c>
-      <c r="F110" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="G110" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H110" t="s">
-        <v>124</v>
-      </c>
-      <c r="I110" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J110" s="3"/>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E111" t="s">
-        <v>145</v>
-      </c>
-      <c r="G111" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="H111" t="s">
-        <v>124</v>
-      </c>
-      <c r="I111" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J111" s="3"/>
-    </row>
-    <row r="112" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E112" t="s">
-        <v>144</v>
-      </c>
-      <c r="G112" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="H112" t="s">
-        <v>124</v>
-      </c>
-      <c r="I112" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J112" s="3"/>
-    </row>
-    <row r="113" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J113" s="3"/>
-    </row>
-    <row r="114" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J114" s="3"/>
-    </row>
-    <row r="115" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J115" s="3"/>
-    </row>
-    <row r="116" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J116" s="3"/>
-    </row>
-    <row r="117" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G116" s="15"/>
+      <c r="I116" s="23"/>
+      <c r="J116" s="13"/>
+    </row>
+    <row r="117" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G117" s="15"/>
+      <c r="I117" s="23"/>
       <c r="J117" s="3"/>
     </row>
-    <row r="118" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I118" s="23"/>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I119" s="23"/>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I120" s="23"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I121" s="23"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I122" s="23"/>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I123" s="23"/>
       <c r="J123" s="3"/>
     </row>
-    <row r="124" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I124" s="23"/>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I125" s="23"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I126" s="23"/>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I127" s="23"/>
       <c r="J127" s="3"/>
     </row>
-    <row r="128" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I128" s="23"/>
       <c r="J128" s="3"/>
     </row>
-    <row r="129" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I129" s="23"/>
       <c r="J129" s="3"/>
     </row>
-    <row r="130" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I130" s="23"/>
       <c r="J130" s="3"/>
     </row>
-    <row r="131" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I131" s="23"/>
       <c r="J131" s="3"/>
     </row>
-    <row r="132" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I132" s="23"/>
       <c r="J132" s="3"/>
     </row>
-    <row r="133" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I133" s="23"/>
       <c r="J133" s="3"/>
     </row>
-    <row r="134" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I134" s="23"/>
       <c r="J134" s="3"/>
     </row>
-    <row r="135" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I135" s="23"/>
       <c r="J135" s="3"/>
     </row>
-    <row r="136" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I136" s="23"/>
       <c r="J136" s="3"/>
     </row>
-    <row r="137" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I137" s="23"/>
       <c r="J137" s="3"/>
     </row>
-    <row r="138" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J138" s="3"/>
     </row>
-    <row r="139" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J139" s="3"/>
     </row>
-    <row r="140" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J140" s="3"/>
     </row>
-    <row r="141" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J141" s="3"/>
     </row>
-    <row r="142" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J142" s="3"/>
     </row>
-    <row r="143" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J143" s="3"/>
     </row>
-    <row r="144" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="9:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J144" s="3"/>
     </row>
     <row r="145" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5197,11 +4948,39 @@
     <row r="1000" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J1000" s="3"/>
     </row>
+    <row r="1001" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1001" s="3"/>
+    </row>
+    <row r="1002" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1002" s="3"/>
+    </row>
+    <row r="1003" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1003" s="3"/>
+    </row>
+    <row r="1004" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1004" s="3"/>
+    </row>
+    <row r="1005" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1005" s="3"/>
+    </row>
+    <row r="1006" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1006" s="3"/>
+    </row>
+    <row r="1007" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1007" s="3"/>
+    </row>
+    <row r="1008" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1008" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I18:I26"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="I42:I44"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1"/>
-    <hyperlink ref="F63" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>